<commit_message>
add secruity + token system
</commit_message>
<xml_diff>
--- a/stock.xlsx
+++ b/stock.xlsx
@@ -154,7 +154,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>6347</v>
+        <v>3468</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -162,7 +162,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>7931</v>
+        <v>5263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>